<commit_message>
publishing blog for feedback
</commit_message>
<xml_diff>
--- a/_languages.xlsx
+++ b/_languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\p2d\l\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B41E52-B595-4982-B29B-938E3CB63F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFE6E62-92EE-4D29-BCE2-ABE873A32B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" tabRatio="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="680">
   <si>
     <t>roman</t>
   </si>
@@ -96,9 +96,6 @@
     <t>ई</t>
   </si>
   <si>
-    <t>īdisa (of such kind)</t>
-  </si>
-  <si>
     <t>ईदिस</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>ऊ</t>
   </si>
   <si>
-    <t>ūhacca (uprooting)</t>
-  </si>
-  <si>
     <t>ऊहच्च</t>
   </si>
   <si>
@@ -1485,36 +1479,12 @@
     <t>07_e_1.short_mettā</t>
   </si>
   <si>
-    <t>ए (short)</t>
-  </si>
-  <si>
-    <t>e (short)</t>
-  </si>
-  <si>
-    <t>e (long)</t>
-  </si>
-  <si>
-    <t>ए (long)</t>
-  </si>
-  <si>
     <t>09_o_1.short_potthaka</t>
   </si>
   <si>
     <t>10_o_2.long_obhāsa</t>
   </si>
   <si>
-    <t>ओ (short)</t>
-  </si>
-  <si>
-    <t>o (short)</t>
-  </si>
-  <si>
-    <t>o (long)</t>
-  </si>
-  <si>
-    <t>ओ (long)</t>
-  </si>
-  <si>
     <t>11_ka_kamma</t>
   </si>
   <si>
@@ -1542,9 +1512,6 @@
     <t>19_jha_jhāna</t>
   </si>
   <si>
-    <t>20_ña_1.begin.option.1_ñāṇa | 20_ña_1.begin.option.2_ñāṇa | 20_ña_2.middle.option.1_paññā | 20_ña_2.middle.option.2_paññā</t>
-  </si>
-  <si>
     <t>21_ṭa_ṭīkā</t>
   </si>
   <si>
@@ -1578,9 +1545,6 @@
     <t>29_dha_dhaja</t>
   </si>
   <si>
-    <t>30_na_1.begin_nibbāna | 30_na_1.middle_khandha</t>
-  </si>
-  <si>
     <t>31_pa_pappoti</t>
   </si>
   <si>
@@ -1623,15 +1587,6 @@
     <t>43_ṁ_saṃsāra</t>
   </si>
   <si>
-    <t>pāḷi</t>
-  </si>
-  <si>
-    <t>पाळि</t>
-  </si>
-  <si>
-    <t>42_ḷa_pāḷi</t>
-  </si>
-  <si>
     <t>01_a</t>
   </si>
   <si>
@@ -2071,6 +2026,45 @@
   </si>
   <si>
     <t>Nasal_vowel</t>
+  </si>
+  <si>
+    <t>30_na_1.begin_nibbāna</t>
+  </si>
+  <si>
+    <t>20_ña_2.middle.option.2_paññā</t>
+  </si>
+  <si>
+    <t>ए (s)</t>
+  </si>
+  <si>
+    <t>ए (l)</t>
+  </si>
+  <si>
+    <t>ओ (s)</t>
+  </si>
+  <si>
+    <t>ओ (l)</t>
+  </si>
+  <si>
+    <t>e (s)</t>
+  </si>
+  <si>
+    <t>e (l)</t>
+  </si>
+  <si>
+    <t>o (s)</t>
+  </si>
+  <si>
+    <t>o (l)</t>
+  </si>
+  <si>
+    <t>saḷāyatana</t>
+  </si>
+  <si>
+    <t>42_ḷa_saḷāyatana</t>
+  </si>
+  <si>
+    <t>सळायतन</t>
   </si>
 </sst>
 </file>
@@ -2704,15 +2698,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="38.46484375" customWidth="1"/>
     <col min="5" max="5" width="9.73046875" customWidth="1"/>
-    <col min="6" max="6" width="17.59765625" customWidth="1"/>
+    <col min="6" max="6" width="56.33203125" customWidth="1"/>
     <col min="7" max="7" width="20.3984375" customWidth="1"/>
     <col min="8" max="8" width="18.265625" customWidth="1"/>
     <col min="10" max="10" width="25.19921875" bestFit="1" customWidth="1"/>
@@ -2741,13 +2736,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>620</v>
+        <v>605</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>604</v>
+        <v>589</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -2758,7 +2753,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -2767,19 +2762,19 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>594</v>
+        <v>579</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>579</v>
+        <v>564</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>595</v>
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -2790,7 +2785,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
@@ -2799,19 +2794,19 @@
         <v>16</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>596</v>
+        <v>581</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>597</v>
+        <v>582</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
@@ -2822,7 +2817,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>19</v>
@@ -2831,19 +2826,19 @@
         <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>598</v>
+        <v>583</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>599</v>
+        <v>584</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
@@ -2854,1276 +2849,1276 @@
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>538</v>
+        <v>523</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>601</v>
+        <v>586</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>600</v>
+        <v>585</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>602</v>
+        <v>587</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>580</v>
+        <v>565</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>603</v>
+        <v>588</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>605</v>
+        <v>590</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>606</v>
+        <v>591</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>487</v>
+        <v>673</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>486</v>
+        <v>669</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>610</v>
+        <v>595</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>607</v>
+        <v>592</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
-        <v>488</v>
+        <v>674</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>489</v>
+        <v>670</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>542</v>
+        <v>527</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>608</v>
+        <v>593</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>581</v>
+        <v>566</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>607</v>
+        <v>592</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
-        <v>493</v>
+        <v>675</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>492</v>
+        <v>671</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>543</v>
+        <v>528</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>611</v>
+        <v>596</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>609</v>
+        <v>594</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
-        <v>494</v>
+        <v>676</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>495</v>
+        <v>672</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>544</v>
+        <v>529</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>612</v>
+        <v>597</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>609</v>
+        <v>594</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>613</v>
+        <v>598</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>657</v>
+        <v>642</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>615</v>
+        <v>600</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>585</v>
+        <v>570</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>614</v>
+        <v>599</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>659</v>
+        <v>644</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>616</v>
+        <v>601</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>586</v>
+        <v>571</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>660</v>
+        <v>645</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>549</v>
+        <v>534</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>617</v>
+        <v>602</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>587</v>
+        <v>572</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>661</v>
+        <v>646</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>618</v>
+        <v>603</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>588</v>
+        <v>573</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>662</v>
+        <v>647</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>502</v>
+        <v>492</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>619</v>
+        <v>604</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>589</v>
+        <v>574</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>621</v>
+        <v>606</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>590</v>
+        <v>575</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>663</v>
+        <v>648</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>622</v>
+        <v>607</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>591</v>
+        <v>576</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>660</v>
+        <v>645</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>505</v>
+        <v>668</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>623</v>
+        <v>608</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>664</v>
+        <v>649</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>624</v>
+        <v>609</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>592</v>
+        <v>577</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>665</v>
+        <v>650</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>625</v>
+        <v>610</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>593</v>
+        <v>578</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>628</v>
+        <v>613</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>626</v>
+        <v>611</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>666</v>
+        <v>651</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>630</v>
+        <v>615</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>629</v>
+        <v>614</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>660</v>
+        <v>645</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>631</v>
+        <v>616</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>667</v>
+        <v>652</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>627</v>
+        <v>612</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>668</v>
+        <v>653</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="F28" s="2" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>634</v>
+        <v>619</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>633</v>
+        <v>618</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>635</v>
+        <v>620</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>669</v>
+        <v>654</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="F30" s="2" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>637</v>
+        <v>622</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>660</v>
+        <v>645</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="F31" s="2" t="s">
-        <v>517</v>
+        <v>667</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>638</v>
+        <v>623</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>670</v>
+        <v>655</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="F32" s="2" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>639</v>
+        <v>624</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="F33" s="2" t="s">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>641</v>
+        <v>626</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>640</v>
+        <v>625</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>642</v>
+        <v>627</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>672</v>
+        <v>657</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="F35" s="2" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>643</v>
+        <v>628</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>644</v>
+        <v>629</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>660</v>
+        <v>645</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>522</v>
+        <v>510</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>645</v>
+        <v>630</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>673</v>
+        <v>658</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>523</v>
+        <v>511</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>646</v>
+        <v>631</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>674</v>
+        <v>659</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>647</v>
+        <v>632</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>583</v>
+        <v>568</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="F39" s="2" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>648</v>
+        <v>633</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>584</v>
+        <v>569</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>676</v>
+        <v>661</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="F40" s="2" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>652</v>
+        <v>637</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>649</v>
+        <v>634</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>677</v>
+        <v>662</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="F41" s="2" t="s">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>650</v>
+        <v>635</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>678</v>
+        <v>663</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="F42" s="2" t="s">
-        <v>528</v>
+        <v>516</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>651</v>
+        <v>636</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>679</v>
+        <v>664</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>576</v>
+        <v>561</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>532</v>
+        <v>677</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>533</v>
+        <v>679</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>534</v>
+        <v>678</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>532</v>
+        <v>677</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>654</v>
+        <v>639</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>653</v>
+        <v>638</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>680</v>
+        <v>665</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>577</v>
+        <v>562</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>530</v>
+        <v>518</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>531</v>
+        <v>519</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>656</v>
+        <v>641</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>655</v>
+        <v>640</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>681</v>
+        <v>666</v>
       </c>
     </row>
   </sheetData>
@@ -4146,67 +4141,67 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>578</v>
+        <v>563</v>
       </c>
     </row>
   </sheetData>
@@ -4234,39 +4229,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" t="s">
         <v>182</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>183</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>184</v>
-      </c>
-      <c r="G1" t="s">
-        <v>185</v>
-      </c>
-      <c r="H1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" t="s">
         <v>187</v>
-      </c>
-      <c r="B2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" t="s">
-        <v>189</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
@@ -4274,181 +4269,181 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" t="s">
         <v>190</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H3" t="s">
         <v>191</v>
-      </c>
-      <c r="D3" t="s">
-        <v>192</v>
-      </c>
-      <c r="H3" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" t="s">
         <v>194</v>
       </c>
-      <c r="B4" t="s">
+      <c r="H4" t="s">
         <v>195</v>
-      </c>
-      <c r="D4" t="s">
-        <v>196</v>
-      </c>
-      <c r="H4" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" t="s">
         <v>198</v>
       </c>
-      <c r="B5" t="s">
+      <c r="H5" t="s">
         <v>199</v>
-      </c>
-      <c r="D5" t="s">
-        <v>200</v>
-      </c>
-      <c r="H5" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" t="s">
         <v>202</v>
       </c>
-      <c r="B6" t="s">
+      <c r="H6" t="s">
         <v>203</v>
-      </c>
-      <c r="D6" t="s">
-        <v>204</v>
-      </c>
-      <c r="H6" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" t="s">
         <v>206</v>
       </c>
-      <c r="B7" t="s">
-        <v>207</v>
-      </c>
-      <c r="D7" t="s">
-        <v>208</v>
-      </c>
       <c r="H7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" t="s">
         <v>209</v>
       </c>
-      <c r="B8" t="s">
+      <c r="H8" t="s">
         <v>210</v>
-      </c>
-      <c r="D8" t="s">
-        <v>211</v>
-      </c>
-      <c r="H8" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" t="s">
         <v>213</v>
       </c>
-      <c r="B9" t="s">
+      <c r="H9" t="s">
         <v>214</v>
-      </c>
-      <c r="D9" t="s">
-        <v>215</v>
-      </c>
-      <c r="H9" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" t="s">
         <v>217</v>
       </c>
-      <c r="B10" t="s">
+      <c r="H10" t="s">
         <v>218</v>
-      </c>
-      <c r="D10" t="s">
-        <v>219</v>
-      </c>
-      <c r="H10" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" t="s">
         <v>221</v>
       </c>
-      <c r="B11" t="s">
+      <c r="H11" t="s">
         <v>222</v>
-      </c>
-      <c r="D11" t="s">
-        <v>223</v>
-      </c>
-      <c r="H11" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12" t="s">
         <v>225</v>
       </c>
-      <c r="B12" t="s">
+      <c r="H12" t="s">
         <v>226</v>
-      </c>
-      <c r="D12" t="s">
-        <v>227</v>
-      </c>
-      <c r="H12" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D13" t="s">
         <v>229</v>
       </c>
-      <c r="B13" t="s">
+      <c r="H13" t="s">
         <v>230</v>
-      </c>
-      <c r="D13" t="s">
-        <v>231</v>
-      </c>
-      <c r="H13" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B14" t="s">
+        <v>232</v>
+      </c>
+      <c r="D14" t="s">
         <v>233</v>
       </c>
-      <c r="B14" t="s">
+      <c r="H14" t="s">
         <v>234</v>
-      </c>
-      <c r="D14" t="s">
-        <v>235</v>
-      </c>
-      <c r="H14" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" t="s">
         <v>237</v>
-      </c>
-      <c r="B15" t="s">
-        <v>238</v>
-      </c>
-      <c r="D15" t="s">
-        <v>239</v>
       </c>
       <c r="H15" t="s">
         <v>12</v>
@@ -4456,475 +4451,475 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" t="s">
+        <v>239</v>
+      </c>
+      <c r="D16" t="s">
         <v>240</v>
       </c>
-      <c r="B16" t="s">
+      <c r="E16" t="s">
         <v>241</v>
       </c>
-      <c r="D16" t="s">
+      <c r="H16" t="s">
         <v>242</v>
-      </c>
-      <c r="E16" t="s">
-        <v>243</v>
-      </c>
-      <c r="H16" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B17" t="s">
+        <v>244</v>
+      </c>
+      <c r="D17" t="s">
         <v>245</v>
       </c>
-      <c r="B17" t="s">
+      <c r="E17" t="s">
         <v>246</v>
       </c>
-      <c r="D17" t="s">
+      <c r="H17" t="s">
         <v>247</v>
-      </c>
-      <c r="E17" t="s">
-        <v>248</v>
-      </c>
-      <c r="H17" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>248</v>
+      </c>
+      <c r="B18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D18" t="s">
         <v>250</v>
       </c>
-      <c r="B18" t="s">
+      <c r="H18" t="s">
         <v>251</v>
-      </c>
-      <c r="D18" t="s">
-        <v>252</v>
-      </c>
-      <c r="H18" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>252</v>
+      </c>
+      <c r="B19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D19" t="s">
         <v>254</v>
       </c>
-      <c r="B19" t="s">
+      <c r="H19" t="s">
         <v>255</v>
-      </c>
-      <c r="D19" t="s">
-        <v>256</v>
-      </c>
-      <c r="H19" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>256</v>
+      </c>
+      <c r="B20" t="s">
+        <v>257</v>
+      </c>
+      <c r="D20" t="s">
         <v>258</v>
       </c>
-      <c r="B20" t="s">
+      <c r="H20" t="s">
         <v>259</v>
-      </c>
-      <c r="D20" t="s">
-        <v>260</v>
-      </c>
-      <c r="H20" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>260</v>
+      </c>
+      <c r="B21" t="s">
+        <v>261</v>
+      </c>
+      <c r="D21" t="s">
         <v>262</v>
       </c>
-      <c r="B21" t="s">
+      <c r="H21" t="s">
         <v>263</v>
-      </c>
-      <c r="D21" t="s">
-        <v>264</v>
-      </c>
-      <c r="H21" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22" t="s">
+        <v>265</v>
+      </c>
+      <c r="D22" t="s">
         <v>266</v>
       </c>
-      <c r="B22" t="s">
+      <c r="H22" t="s">
         <v>267</v>
-      </c>
-      <c r="D22" t="s">
-        <v>268</v>
-      </c>
-      <c r="H22" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
+        <v>268</v>
+      </c>
+      <c r="B23" t="s">
+        <v>269</v>
+      </c>
+      <c r="D23" t="s">
         <v>270</v>
       </c>
-      <c r="B23" t="s">
+      <c r="H23" t="s">
         <v>271</v>
-      </c>
-      <c r="D23" t="s">
-        <v>272</v>
-      </c>
-      <c r="H23" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
+        <v>272</v>
+      </c>
+      <c r="B24" t="s">
+        <v>273</v>
+      </c>
+      <c r="D24" t="s">
         <v>274</v>
       </c>
-      <c r="B24" t="s">
-        <v>275</v>
-      </c>
-      <c r="D24" t="s">
-        <v>276</v>
-      </c>
       <c r="H24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>275</v>
+      </c>
+      <c r="B25" t="s">
+        <v>276</v>
+      </c>
+      <c r="D25" t="s">
         <v>277</v>
       </c>
-      <c r="B25" t="s">
+      <c r="H25" t="s">
         <v>278</v>
-      </c>
-      <c r="D25" t="s">
-        <v>279</v>
-      </c>
-      <c r="H25" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
+        <v>279</v>
+      </c>
+      <c r="B26" t="s">
+        <v>280</v>
+      </c>
+      <c r="D26" t="s">
         <v>281</v>
       </c>
-      <c r="B26" t="s">
+      <c r="H26" t="s">
         <v>282</v>
-      </c>
-      <c r="D26" t="s">
-        <v>283</v>
-      </c>
-      <c r="H26" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
+        <v>283</v>
+      </c>
+      <c r="B27" t="s">
+        <v>284</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" t="s">
         <v>285</v>
       </c>
-      <c r="B27" t="s">
-        <v>286</v>
-      </c>
-      <c r="D27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" t="s">
-        <v>287</v>
-      </c>
       <c r="H27" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
+        <v>286</v>
+      </c>
+      <c r="B28" t="s">
+        <v>287</v>
+      </c>
+      <c r="D28" t="s">
         <v>288</v>
       </c>
-      <c r="B28" t="s">
+      <c r="H28" t="s">
         <v>289</v>
-      </c>
-      <c r="D28" t="s">
-        <v>290</v>
-      </c>
-      <c r="H28" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
+        <v>290</v>
+      </c>
+      <c r="B29" t="s">
+        <v>291</v>
+      </c>
+      <c r="D29" t="s">
         <v>292</v>
       </c>
-      <c r="B29" t="s">
+      <c r="E29" t="s">
         <v>293</v>
       </c>
-      <c r="D29" t="s">
+      <c r="H29" t="s">
         <v>294</v>
-      </c>
-      <c r="E29" t="s">
-        <v>295</v>
-      </c>
-      <c r="H29" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>295</v>
+      </c>
+      <c r="B30" t="s">
+        <v>296</v>
+      </c>
+      <c r="D30" t="s">
         <v>297</v>
       </c>
-      <c r="B30" t="s">
+      <c r="H30" t="s">
         <v>298</v>
-      </c>
-      <c r="D30" t="s">
-        <v>299</v>
-      </c>
-      <c r="H30" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>299</v>
+      </c>
+      <c r="B31" t="s">
+        <v>300</v>
+      </c>
+      <c r="D31" t="s">
         <v>301</v>
       </c>
-      <c r="B31" t="s">
+      <c r="H31" t="s">
         <v>302</v>
-      </c>
-      <c r="D31" t="s">
-        <v>303</v>
-      </c>
-      <c r="H31" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>303</v>
+      </c>
+      <c r="B32" t="s">
+        <v>304</v>
+      </c>
+      <c r="D32" t="s">
         <v>305</v>
       </c>
-      <c r="B32" t="s">
+      <c r="H32" t="s">
         <v>306</v>
-      </c>
-      <c r="D32" t="s">
-        <v>307</v>
-      </c>
-      <c r="H32" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
+        <v>307</v>
+      </c>
+      <c r="B33" t="s">
+        <v>308</v>
+      </c>
+      <c r="D33" t="s">
         <v>309</v>
       </c>
-      <c r="B33" t="s">
+      <c r="H33" t="s">
         <v>310</v>
-      </c>
-      <c r="D33" t="s">
-        <v>311</v>
-      </c>
-      <c r="H33" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>311</v>
+      </c>
+      <c r="B34" t="s">
+        <v>312</v>
+      </c>
+      <c r="D34" t="s">
         <v>313</v>
       </c>
-      <c r="B34" t="s">
-        <v>314</v>
-      </c>
-      <c r="D34" t="s">
-        <v>315</v>
-      </c>
       <c r="H34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>314</v>
+      </c>
+      <c r="B35" t="s">
+        <v>315</v>
+      </c>
+      <c r="D35" t="s">
         <v>316</v>
       </c>
-      <c r="B35" t="s">
+      <c r="H35" t="s">
         <v>317</v>
-      </c>
-      <c r="D35" t="s">
-        <v>318</v>
-      </c>
-      <c r="H35" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B36" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D36" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H36" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>320</v>
+      </c>
+      <c r="B37" t="s">
+        <v>321</v>
+      </c>
+      <c r="D37" t="s">
         <v>322</v>
       </c>
-      <c r="B37" t="s">
+      <c r="H37" t="s">
         <v>323</v>
-      </c>
-      <c r="D37" t="s">
-        <v>324</v>
-      </c>
-      <c r="H37" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
+        <v>324</v>
+      </c>
+      <c r="B38" t="s">
+        <v>325</v>
+      </c>
+      <c r="D38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" t="s">
         <v>326</v>
       </c>
-      <c r="B38" t="s">
-        <v>327</v>
-      </c>
-      <c r="D38" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" t="s">
-        <v>328</v>
-      </c>
       <c r="H38" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
+        <v>327</v>
+      </c>
+      <c r="B39" t="s">
+        <v>328</v>
+      </c>
+      <c r="D39" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" t="s">
         <v>329</v>
       </c>
-      <c r="B39" t="s">
-        <v>330</v>
-      </c>
-      <c r="D39" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" t="s">
-        <v>331</v>
-      </c>
       <c r="H39" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
+        <v>330</v>
+      </c>
+      <c r="B40" t="s">
+        <v>331</v>
+      </c>
+      <c r="D40" t="s">
+        <v>240</v>
+      </c>
+      <c r="E40" t="s">
         <v>332</v>
       </c>
-      <c r="B40" t="s">
-        <v>333</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="H40" t="s">
         <v>242</v>
-      </c>
-      <c r="E40" t="s">
-        <v>334</v>
-      </c>
-      <c r="H40" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
+        <v>333</v>
+      </c>
+      <c r="B41" t="s">
+        <v>334</v>
+      </c>
+      <c r="D41" t="s">
+        <v>245</v>
+      </c>
+      <c r="E41" t="s">
         <v>335</v>
       </c>
-      <c r="B41" t="s">
-        <v>336</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="H41" t="s">
         <v>247</v>
-      </c>
-      <c r="E41" t="s">
-        <v>337</v>
-      </c>
-      <c r="H41" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B42" t="s">
+        <v>337</v>
+      </c>
+      <c r="D42" t="s">
         <v>338</v>
       </c>
-      <c r="B42" t="s">
+      <c r="H42" t="s">
         <v>339</v>
-      </c>
-      <c r="D42" t="s">
-        <v>340</v>
-      </c>
-      <c r="H42" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
+        <v>340</v>
+      </c>
+      <c r="B43" t="s">
+        <v>341</v>
+      </c>
+      <c r="D43" t="s">
         <v>342</v>
       </c>
-      <c r="B43" t="s">
+      <c r="H43" t="s">
         <v>343</v>
-      </c>
-      <c r="D43" t="s">
-        <v>344</v>
-      </c>
-      <c r="H43" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
+        <v>344</v>
+      </c>
+      <c r="B44" t="s">
+        <v>345</v>
+      </c>
+      <c r="D44" t="s">
         <v>346</v>
       </c>
-      <c r="B44" t="s">
+      <c r="E44" t="s">
+        <v>329</v>
+      </c>
+      <c r="F44" t="s">
         <v>347</v>
       </c>
-      <c r="D44" t="s">
+      <c r="H44" t="s">
         <v>348</v>
-      </c>
-      <c r="E44" t="s">
-        <v>331</v>
-      </c>
-      <c r="F44" t="s">
-        <v>349</v>
-      </c>
-      <c r="H44" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
+        <v>349</v>
+      </c>
+      <c r="B45" t="s">
+        <v>350</v>
+      </c>
+      <c r="D45" t="s">
         <v>351</v>
       </c>
-      <c r="B45" t="s">
+      <c r="F45" t="s">
+        <v>347</v>
+      </c>
+      <c r="H45" t="s">
         <v>352</v>
-      </c>
-      <c r="D45" t="s">
-        <v>353</v>
-      </c>
-      <c r="F45" t="s">
-        <v>349</v>
-      </c>
-      <c r="H45" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
+        <v>353</v>
+      </c>
+      <c r="B46" t="s">
+        <v>354</v>
+      </c>
+      <c r="D46" t="s">
         <v>355</v>
       </c>
-      <c r="B46" t="s">
+      <c r="E46" t="s">
+        <v>329</v>
+      </c>
+      <c r="F46" t="s">
+        <v>347</v>
+      </c>
+      <c r="H46" t="s">
         <v>356</v>
-      </c>
-      <c r="D46" t="s">
-        <v>357</v>
-      </c>
-      <c r="E46" t="s">
-        <v>331</v>
-      </c>
-      <c r="F46" t="s">
-        <v>349</v>
-      </c>
-      <c r="H46" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -4951,75 +4946,75 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1" t="s">
         <v>359</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>360</v>
       </c>
-      <c r="C1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D1" t="s">
-        <v>362</v>
-      </c>
       <c r="E1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -5049,557 +5044,557 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1" t="s">
         <v>360</v>
       </c>
-      <c r="C1" t="s">
-        <v>362</v>
-      </c>
       <c r="D1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C2" t="s">
         <v>373</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>374</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>375</v>
-      </c>
-      <c r="D2" t="s">
-        <v>376</v>
-      </c>
-      <c r="E2" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C3" t="s">
         <v>378</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>379</v>
-      </c>
-      <c r="C3" t="s">
-        <v>380</v>
-      </c>
-      <c r="D3" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C4" t="s">
         <v>382</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>383</v>
-      </c>
-      <c r="C4" t="s">
-        <v>384</v>
-      </c>
-      <c r="D4" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>384</v>
+      </c>
+      <c r="B5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" t="s">
         <v>386</v>
       </c>
-      <c r="B5" t="s">
-        <v>387</v>
-      </c>
-      <c r="C5" t="s">
-        <v>388</v>
-      </c>
       <c r="D5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>387</v>
+      </c>
+      <c r="B6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C6" t="s">
         <v>389</v>
       </c>
-      <c r="B6" t="s">
-        <v>390</v>
-      </c>
-      <c r="C6" t="s">
-        <v>391</v>
-      </c>
       <c r="D6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C8" t="s">
         <v>394</v>
       </c>
-      <c r="B8" t="s">
-        <v>395</v>
-      </c>
-      <c r="C8" t="s">
-        <v>396</v>
-      </c>
       <c r="D8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B9" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D9" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C10" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B11" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C11" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D11" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B12" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D12" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B13" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B14" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B15" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D15" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B16" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D16" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B17" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D17" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B18" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D18" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B19" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D19" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B20" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D20" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B21" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D21" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B22" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D22" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B23" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D23" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B24" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D24" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B25" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D25" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B26" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D26" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B27" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D27" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B28" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D28" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D29" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E29" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D30" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E30" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E31" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D32" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E32" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B33" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D33" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B34" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D34" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D35" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E35" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D36" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E36" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D38" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B39" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D39" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D40" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B41" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D41" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B42" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D42" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D43" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B45" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D45" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B46" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D46" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -5622,39 +5617,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feedback from v bdhrs
</commit_message>
<xml_diff>
--- a/_languages.xlsx
+++ b/_languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\p2d\l\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CE3D18-81C0-45AF-B53E-F9E1AFD1AA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916F60BD-EC96-47CB-B08D-5AF4FBBB7C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" tabRatio="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="671">
   <si>
     <t>roman</t>
   </si>
@@ -1674,9 +1674,6 @@
     <t>43_ṁ</t>
   </si>
   <si>
-    <t>ɐ</t>
-  </si>
-  <si>
     <t>ʊ</t>
   </si>
   <si>
@@ -1719,15 +1716,6 @@
     <t>ʈʰ</t>
   </si>
   <si>
-    <t>a in comma</t>
-  </si>
-  <si>
-    <t>Near-open_central_vowel</t>
-  </si>
-  <si>
-    <t>a in bra</t>
-  </si>
-  <si>
     <t>Open_front_unrounded_vowel</t>
   </si>
   <si>
@@ -1767,12 +1755,6 @@
     <t>Close-mid_back_rounded_vowel</t>
   </si>
   <si>
-    <t>&lt;half of long-e&gt;</t>
-  </si>
-  <si>
-    <t>&lt;half of long-o&gt;</t>
-  </si>
-  <si>
     <t>o in old</t>
   </si>
   <si>
@@ -1782,9 +1764,6 @@
     <t>g in again</t>
   </si>
   <si>
-    <t>kh in khan</t>
-  </si>
-  <si>
     <t>gh in doghouse</t>
   </si>
   <si>
@@ -1899,15 +1878,9 @@
     <t>l̩</t>
   </si>
   <si>
-    <t>le in bottle</t>
-  </si>
-  <si>
     <t>◌̃</t>
   </si>
   <si>
-    <t>&lt;nasal vowel&gt;</t>
-  </si>
-  <si>
     <t>Voiceless_velar_plosive</t>
   </si>
   <si>
@@ -2029,6 +2002,42 @@
   </si>
   <si>
     <t>पञ्ञा</t>
+  </si>
+  <si>
+    <t>s dovolením</t>
+  </si>
+  <si>
+    <t>pardon</t>
+  </si>
+  <si>
+    <t>excuse me / sorry (e.g. bumped into someone)</t>
+  </si>
+  <si>
+    <t>u in cut / hut</t>
+  </si>
+  <si>
+    <t>a in bra / father</t>
+  </si>
+  <si>
+    <t>l in girl</t>
+  </si>
+  <si>
+    <t>ng in sing</t>
+  </si>
+  <si>
+    <t>ə</t>
+  </si>
+  <si>
+    <t>Mid_central_vowel</t>
+  </si>
+  <si>
+    <t>e in met / bed</t>
+  </si>
+  <si>
+    <t>o in short</t>
+  </si>
+  <si>
+    <t>kh in backhand</t>
   </si>
 </sst>
 </file>
@@ -2349,8 +2358,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6594609-297C-40F6-AF66-042A98E3F884}" name="Table5" displayName="Table5" ref="A1:F48" totalsRowShown="0">
-  <autoFilter ref="A1:F48" xr:uid="{C6594609-297C-40F6-AF66-042A98E3F884}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6594609-297C-40F6-AF66-042A98E3F884}" name="Table5" displayName="Table5" ref="A1:F49" totalsRowShown="0">
+  <autoFilter ref="A1:F49" xr:uid="{C6594609-297C-40F6-AF66-042A98E3F884}"/>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{097E607D-45C3-40C4-B92E-E44E827F015E}" name="česky"/>
     <tableColumn id="3" xr3:uid="{75EC0192-22C5-4FDD-95A8-6A9B2EEF665A}" name="mic"/>
@@ -2662,8 +2671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2700,13 +2709,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -2732,13 +2741,13 @@
         <v>440</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>564</v>
+        <v>662</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>549</v>
+        <v>666</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>565</v>
+        <v>667</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -2764,13 +2773,13 @@
         <v>441</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>566</v>
+        <v>663</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>177</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
@@ -2796,13 +2805,13 @@
         <v>19</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>228</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
@@ -2828,13 +2837,13 @@
         <v>442</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>233</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
@@ -2860,13 +2869,13 @@
         <v>26</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
@@ -2892,21 +2901,21 @@
         <v>443</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>303</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>512</v>
@@ -2924,21 +2933,21 @@
         <v>34</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>580</v>
+        <v>668</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>513</v>
@@ -2956,21 +2965,21 @@
         <v>444</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>514</v>
@@ -2988,21 +2997,21 @@
         <v>39</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>581</v>
+        <v>669</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>36</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
-        <v>661</v>
+        <v>652</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>515</v>
@@ -3020,13 +3029,13 @@
         <v>37</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>264</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
@@ -3052,13 +3061,13 @@
         <v>445</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>241</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
@@ -3084,13 +3093,13 @@
         <v>446</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>585</v>
+        <v>670</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
@@ -3116,13 +3125,13 @@
         <v>51</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>216</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
@@ -3148,13 +3157,13 @@
         <v>55</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
@@ -3180,13 +3189,13 @@
         <v>449</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>631</v>
+        <v>622</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
@@ -3212,13 +3221,13 @@
         <v>448</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
@@ -3244,13 +3253,13 @@
         <v>66</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
@@ -3276,13 +3285,13 @@
         <v>449</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
@@ -3308,13 +3317,13 @@
         <v>74</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
@@ -3328,25 +3337,25 @@
         <v>525</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>667</v>
+        <v>658</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>666</v>
+        <v>657</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>257</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
@@ -3372,13 +3381,13 @@
         <v>80</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
@@ -3404,13 +3413,13 @@
         <v>450</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
@@ -3436,13 +3445,13 @@
         <v>451</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
@@ -3468,13 +3477,13 @@
         <v>452</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
@@ -3500,13 +3509,13 @@
         <v>453</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>637</v>
+        <v>628</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
@@ -3532,13 +3541,13 @@
         <v>98</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>292</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
@@ -3564,13 +3573,13 @@
         <v>454</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
@@ -3596,13 +3605,13 @@
         <v>455</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>163</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
@@ -3628,13 +3637,13 @@
         <v>456</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
@@ -3654,19 +3663,19 @@
         <v>114</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>113</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>348</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
@@ -3692,13 +3701,13 @@
         <v>117</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>268</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
@@ -3724,13 +3733,13 @@
         <v>457</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
@@ -3756,13 +3765,13 @@
         <v>125</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>181</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
@@ -3788,13 +3797,13 @@
         <v>129</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
@@ -3820,13 +3829,13 @@
         <v>133</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
@@ -3852,13 +3861,13 @@
         <v>458</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>237</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
@@ -3884,13 +3893,13 @@
         <v>459</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
@@ -3916,13 +3925,13 @@
         <v>460</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
@@ -3948,13 +3957,13 @@
         <v>461</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
@@ -3980,13 +3989,13 @@
         <v>447</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>284</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
@@ -4012,13 +4021,13 @@
         <v>157</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>220</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>649</v>
+        <v>640</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
@@ -4032,25 +4041,25 @@
         <v>547</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
       <c r="E43" s="9" t="s">
+        <v>655</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="F43" s="9" t="s">
-        <v>663</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>662</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>624</v>
-      </c>
       <c r="I43" s="2" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
@@ -4076,13 +4085,13 @@
         <v>503</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>626</v>
+        <v>665</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -4925,10 +4934,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABB4F22-6F20-44EB-B543-DE5FAB802FCF}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5434,7 +5443,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>659</v>
       </c>
       <c r="B40" t="s">
         <v>425</v>
@@ -5445,53 +5454,64 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>426</v>
+        <v>660</v>
       </c>
       <c r="B41" t="s">
-        <v>427</v>
+        <v>661</v>
       </c>
       <c r="D41" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
+        <v>426</v>
+      </c>
+      <c r="B42" t="s">
+        <v>427</v>
+      </c>
+      <c r="D42" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>428</v>
       </c>
-      <c r="B42" t="s">
-        <v>429</v>
-      </c>
-      <c r="D42" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
         <v>429</v>
       </c>
       <c r="D43" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B44" t="s">
+        <v>429</v>
+      </c>
+      <c r="D44" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>430</v>
-      </c>
-      <c r="B45" t="s">
-        <v>431</v>
-      </c>
-      <c r="D45" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
+        <v>430</v>
+      </c>
+      <c r="B46" t="s">
+        <v>431</v>
+      </c>
+      <c r="D46" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
         <v>432</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>405</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>369</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final round of feedback on pāli stuff
</commit_message>
<xml_diff>
--- a/_languages.xlsx
+++ b/_languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\p2d\l\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916F60BD-EC96-47CB-B08D-5AF4FBBB7C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362E584C-1F06-4B93-97FC-08D80BD3F67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" tabRatio="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,12 +57,6 @@
     <t>अ</t>
   </si>
   <si>
-    <t>arahanta</t>
-  </si>
-  <si>
-    <t>अरहन्त</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -72,63 +66,33 @@
     <t>आ</t>
   </si>
   <si>
-    <t>āyatana</t>
-  </si>
-  <si>
-    <t>आयतन</t>
-  </si>
-  <si>
     <t>i</t>
   </si>
   <si>
     <t>इ</t>
   </si>
   <si>
-    <t>icchā</t>
-  </si>
-  <si>
-    <t>इच्छा</t>
-  </si>
-  <si>
     <t>ī</t>
   </si>
   <si>
     <t>ई</t>
   </si>
   <si>
-    <t>ईदिस</t>
-  </si>
-  <si>
     <t>u</t>
   </si>
   <si>
     <t>उ</t>
   </si>
   <si>
-    <t>uposatha</t>
-  </si>
-  <si>
-    <t>उपोसथ</t>
-  </si>
-  <si>
     <t>ū</t>
   </si>
   <si>
     <t>ऊ</t>
   </si>
   <si>
-    <t>ऊहच्च</t>
-  </si>
-  <si>
     <t>e</t>
   </si>
   <si>
-    <t>eka</t>
-  </si>
-  <si>
-    <t>एक</t>
-  </si>
-  <si>
     <t>mettā</t>
   </si>
   <si>
@@ -138,12 +102,6 @@
     <t>o</t>
   </si>
   <si>
-    <t>obhāsa</t>
-  </si>
-  <si>
-    <t>ओभास</t>
-  </si>
-  <si>
     <t>potthaka</t>
   </si>
   <si>
@@ -1347,21 +1305,6 @@
     <t>https://youtu.be/WLf7l15K9R4?t=489</t>
   </si>
   <si>
-    <t>arahant</t>
-  </si>
-  <si>
-    <t>āyatana 1</t>
-  </si>
-  <si>
-    <t>īdisa</t>
-  </si>
-  <si>
-    <t>ūhacca</t>
-  </si>
-  <si>
-    <t>eka 1</t>
-  </si>
-  <si>
     <t>kamma 1</t>
   </si>
   <si>
@@ -1413,36 +1356,12 @@
     <t>viveka 2</t>
   </si>
   <si>
-    <t>01_a_arahanta</t>
-  </si>
-  <si>
-    <t>02_ā_āyatana</t>
-  </si>
-  <si>
-    <t>03_i_icchā</t>
-  </si>
-  <si>
-    <t>04_ī_īdisa</t>
-  </si>
-  <si>
-    <t>05_u_uposatha</t>
-  </si>
-  <si>
-    <t>06_ū_ūhacca</t>
-  </si>
-  <si>
-    <t>08_e_2.long_eka</t>
-  </si>
-  <si>
     <t>07_e_1.short_mettā</t>
   </si>
   <si>
     <t>09_o_1.short_potthaka</t>
   </si>
   <si>
-    <t>10_o_2.long_obhāsa</t>
-  </si>
-  <si>
     <t>11_ka_kamma</t>
   </si>
   <si>
@@ -1878,9 +1797,6 @@
     <t>l̩</t>
   </si>
   <si>
-    <t>◌̃</t>
-  </si>
-  <si>
     <t>Voiceless_velar_plosive</t>
   </si>
   <si>
@@ -1953,9 +1869,6 @@
     <t>Syllabic_consonant</t>
   </si>
   <si>
-    <t>Nasal_vowel</t>
-  </si>
-  <si>
     <t>30_na_1.begin_nibbāna</t>
   </si>
   <si>
@@ -2022,9 +1935,6 @@
     <t>l in girl</t>
   </si>
   <si>
-    <t>ng in sing</t>
-  </si>
-  <si>
     <t>ə</t>
   </si>
   <si>
@@ -2038,25 +1948,109 @@
   </si>
   <si>
     <t>kh in backhand</t>
+  </si>
+  <si>
+    <t>samaṇa 1</t>
+  </si>
+  <si>
+    <t>01_a_samaṇa</t>
+  </si>
+  <si>
+    <t>samaṇa</t>
+  </si>
+  <si>
+    <t>समण</t>
+  </si>
+  <si>
+    <t>02_ā_samādhi</t>
+  </si>
+  <si>
+    <t>samādhi</t>
+  </si>
+  <si>
+    <t>समाधि</t>
+  </si>
+  <si>
+    <t>10_o_2.long_soka</t>
+  </si>
+  <si>
+    <t>soka</t>
+  </si>
+  <si>
+    <t>सोक</t>
+  </si>
+  <si>
+    <t>08_e_2.long_kevala</t>
+  </si>
+  <si>
+    <t>kevala 1</t>
+  </si>
+  <si>
+    <t>kevala</t>
+  </si>
+  <si>
+    <t>केवल</t>
+  </si>
+  <si>
+    <t>kūṭa</t>
+  </si>
+  <si>
+    <t>06_ū_kūṭa</t>
+  </si>
+  <si>
+    <t>kūṭa 1</t>
+  </si>
+  <si>
+    <t>kula</t>
+  </si>
+  <si>
+    <t>05_u_kula</t>
+  </si>
+  <si>
+    <t>kula 1</t>
+  </si>
+  <si>
+    <t>कुल</t>
+  </si>
+  <si>
+    <t>कूट</t>
+  </si>
+  <si>
+    <t>03_i_pati</t>
+  </si>
+  <si>
+    <t>pati 3</t>
+  </si>
+  <si>
+    <t>pati</t>
+  </si>
+  <si>
+    <t>पति</t>
+  </si>
+  <si>
+    <t>04_ī_atīta</t>
+  </si>
+  <si>
+    <t>atīta 1</t>
+  </si>
+  <si>
+    <t>atīta</t>
+  </si>
+  <si>
+    <t>अतीत</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2093,24 +2087,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor theme="8" tint="0.79998168889431442"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -2148,26 +2130,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2672,12 +2649,12 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="3" max="3" width="26.796875" customWidth="1"/>
     <col min="4" max="4" width="38.46484375" customWidth="1"/>
     <col min="5" max="5" width="9.73046875" customWidth="1"/>
     <col min="6" max="6" width="56.33203125" customWidth="1"/>
@@ -2709,1389 +2686,1389 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>583</v>
+        <v>556</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>647</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="I28" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="D29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>463</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H38" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="H39" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="8" t="s">
-        <v>649</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>645</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>512</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="7" t="s">
-        <v>650</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>646</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>468</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>647</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>514</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>470</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>669</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="7" t="s">
-        <v>652</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>648</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>471</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>576</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="H40" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="D41" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="G41" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="D42" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="G42" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A43" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="7" t="s">
+      <c r="D43" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A44" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="E44" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="F44" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>644</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>589</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A25" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="G44" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>593</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A26" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="I26" s="2" t="s">
+      <c r="J44" s="1" t="s">
         <v>594</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A28" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A31" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A34" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A35" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A36" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A37" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A38" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A39" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A40" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A41" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A42" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A43" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>547</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>655</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>654</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>664</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A44" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>548</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>503</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>504</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>505</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>503</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>665</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -4136,39 +4113,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="G1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="H1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
@@ -4176,661 +4153,661 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="H3" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="H4" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="H5" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="H6" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="H7" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B8" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="D8" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="H8" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="D9" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="H9" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="H10" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="H11" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="D12" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="H12" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B13" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="D13" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="H13" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B14" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="D14" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="H14" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="D15" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="H15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="B16" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="D16" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="E16" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="H16" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B17" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="D17" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="E17" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H17" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B18" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="D18" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="H18" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="B19" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="D19" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="H19" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B20" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="D20" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="H20" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B21" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="D21" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="H21" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B22" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="D22" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="H22" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B23" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="D23" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="H23" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B24" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="D24" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="H24" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="B25" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="D25" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="H25" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="B26" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="D26" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="H26" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="B27" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="H27" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="B28" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="D28" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="H28" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="B29" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="D29" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="E29" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="H29" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="B30" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="D30" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="H30" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="B31" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="D31" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="H31" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B32" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="D32" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="H32" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="B33" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="D33" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="H33" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B34" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="D34" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="H34" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B35" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="D35" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="H35" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="B36" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="D36" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="H36" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="B37" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="D37" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="H37" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="B38" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E38" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="H38" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="B39" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="D39" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="H39" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="B40" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="D40" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="E40" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="H40" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="B41" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="D41" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="E41" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="H41" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="B42" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="D42" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="H42" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="B43" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="D43" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="H43" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="B44" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="D44" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="E44" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="F44" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="H44" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="B45" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="D45" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="F45" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="H45" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="B46" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="D46" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="E46" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="F46" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="H46" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -4853,75 +4830,75 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="B1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="C1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="D1" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="E1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="C2" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C3" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="C4" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="C5" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="C6" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="C7" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="C8" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -4951,568 +4928,568 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="B1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="C1" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="D1" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="E1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="F1" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="B2" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="C2" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="D2" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="E2" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="B3" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="C3" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="D3" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="B4" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="C4" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="D4" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="B5" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="C5" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="D5" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="B6" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="C6" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="D6" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="B7" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="C7" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="D7" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="B8" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="C8" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="D8" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="B9" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="C9" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="D9" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="B10" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="C10" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="D10" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="B11" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="C11" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="D11" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="B12" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="C12" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="D12" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="B13" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="D13" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="B14" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="D14" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="B15" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="D15" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B16" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="D16" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="B17" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="D17" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="B18" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="D18" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B19" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="D19" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="B20" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="D20" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="B21" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="D21" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="B22" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="D22" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="B23" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="D23" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="B24" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="D24" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="B25" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="D25" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="B26" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="D26" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="B27" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="D27" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="B28" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="D28" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="D29" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="E29" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="D30" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="E30" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="D31" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="E31" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="D32" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="E32" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="B33" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="D33" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="B34" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="D34" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="D35" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="E35" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="D36" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="E36" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D37" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="D38" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="B39" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="D39" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>659</v>
+        <v>630</v>
       </c>
       <c r="B40" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="D40" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>660</v>
+        <v>631</v>
       </c>
       <c r="B41" t="s">
-        <v>661</v>
+        <v>632</v>
       </c>
       <c r="D41" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="B42" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="D42" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="B43" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="D43" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="D44" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="B46" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="D46" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="B47" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="D47" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -5535,39 +5512,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B1" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>437</v>
+      <c r="A7" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>438</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>439</v>
+        <v>424</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>